<commit_message>
adding the import past
</commit_message>
<xml_diff>
--- a/public/data/roster_data.xlsx
+++ b/public/data/roster_data.xlsx
@@ -431,85 +431,85 @@
         <v>Remark</v>
       </c>
       <c r="J1" t="str">
-        <v/>
+        <v>From</v>
       </c>
       <c r="K1" t="str">
-        <v>From</v>
+        <v>STD(L)</v>
       </c>
       <c r="L1" t="str">
-        <v>STD(L)</v>
+        <v>STD(Z)</v>
       </c>
       <c r="M1" t="str">
-        <v>STD(Z)</v>
+        <v>To</v>
       </c>
       <c r="N1" t="str">
-        <v>To</v>
+        <v>STA(L)</v>
       </c>
       <c r="O1" t="str">
-        <v>STA(L)</v>
+        <v>STA(Z)</v>
       </c>
       <c r="P1" t="str">
-        <v>STA(Z)</v>
+        <v>AC/Hotel</v>
       </c>
       <c r="Q1" t="str">
-        <v>AC/Hotel</v>
+        <v>BLH</v>
       </c>
       <c r="R1" t="str">
-        <v>BLH</v>
+        <v>Flight Time</v>
       </c>
       <c r="S1" t="str">
-        <v>Flight Time</v>
+        <v>Night Time</v>
       </c>
       <c r="T1" t="str">
-        <v>Night Time</v>
+        <v>Dur</v>
       </c>
       <c r="U1" t="str">
-        <v>Dur</v>
+        <v>Ext</v>
       </c>
       <c r="V1" t="str">
-        <v>Ext</v>
+        <v>Pax booked</v>
       </c>
       <c r="W1" t="str">
-        <v>Pax booked</v>
+        <v>ACReg</v>
       </c>
       <c r="X1" t="str">
-        <v>ACReg</v>
+        <v>CrewMeal</v>
       </c>
       <c r="Y1" t="str">
-        <v>CrewMeal</v>
+        <v>Resources</v>
       </c>
       <c r="Z1" t="str">
-        <v>Resources</v>
+        <v>CC</v>
       </c>
       <c r="AA1" t="str">
-        <v>CC</v>
+        <v>Name</v>
       </c>
       <c r="AB1" t="str">
-        <v>Name</v>
+        <v>Pos.</v>
       </c>
       <c r="AC1" t="str">
-        <v>Pos.</v>
+        <v>Work Phone</v>
       </c>
       <c r="AD1" t="str">
-        <v>Work Phone</v>
+        <v>DH Crew</v>
       </c>
       <c r="AE1" t="str">
-        <v>DH Crew</v>
+        <v>DH Name</v>
       </c>
       <c r="AF1" t="str">
-        <v>DH Name</v>
+        <v>DH Seat</v>
       </c>
       <c r="AG1" t="str">
-        <v>DH Seat</v>
+        <v>Remarks</v>
       </c>
       <c r="AH1" t="str">
-        <v>Remarks</v>
+        <v>Fdp Time</v>
       </c>
       <c r="AI1" t="str">
-        <v>Fdp Time</v>
+        <v>Max Fdp</v>
       </c>
       <c r="AJ1" t="str">
-        <v>Max Fdp</v>
+        <v/>
       </c>
       <c r="AK1" t="str">
         <v>Rest Compl.</v>
@@ -544,28 +544,28 @@
         <v>DX 0077</v>
       </c>
       <c r="J2" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K2" t="str">
-        <v>KRP</v>
+        <v>0945</v>
       </c>
       <c r="L2" t="str">
-        <v>0945</v>
+        <v>0845</v>
       </c>
       <c r="M2" t="str">
-        <v>0845</v>
+        <v>CPH</v>
       </c>
       <c r="N2" t="str">
-        <v>CPH</v>
+        <v>1035</v>
       </c>
       <c r="O2" t="str">
-        <v>1035</v>
+        <v>0935</v>
       </c>
       <c r="P2" t="str">
-        <v>0935</v>
+        <v>DO4</v>
       </c>
       <c r="Q2" t="str">
-        <v>DO4</v>
+        <v/>
       </c>
       <c r="R2" t="str">
         <v/>
@@ -598,10 +598,10 @@
         <v>JBNTHIILV</v>
       </c>
       <c r="AB2" t="str">
-        <v/>
+        <v>CP (PIC)FOCA</v>
       </c>
       <c r="AC2" t="str">
-        <v>CP (PIC)FOCA</v>
+        <v/>
       </c>
       <c r="AD2" t="str">
         <v/>
@@ -648,16 +648,16 @@
         <v/>
       </c>
       <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
         <v>DX80</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>DX 0080</v>
       </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
       <c r="J3" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K3" t="str">
         <v>1445</v>
@@ -666,7 +666,7 @@
         <v>1345</v>
       </c>
       <c r="M3" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N3" t="str">
         <v>1535</v>
@@ -675,7 +675,7 @@
         <v>1435</v>
       </c>
       <c r="P3" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q3" t="str">
         <v/>
@@ -761,16 +761,16 @@
         <v/>
       </c>
       <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
         <v>DX83</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <v>DX 0083</v>
       </c>
-      <c r="I4" t="str">
-        <v/>
-      </c>
       <c r="J4" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K4" t="str">
         <v>1620</v>
@@ -779,7 +779,7 @@
         <v>1520</v>
       </c>
       <c r="M4" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="N4" t="str">
         <v>1710</v>
@@ -788,7 +788,7 @@
         <v>1610</v>
       </c>
       <c r="P4" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q4" t="str">
         <v/>
@@ -868,22 +868,22 @@
         <v/>
       </c>
       <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
         <v>1855</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" t="str">
         <v>1755</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <v>DX82</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <v>DX 0082</v>
       </c>
-      <c r="I5" t="str">
-        <v/>
-      </c>
       <c r="J5" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K5" t="str">
         <v>1745</v>
@@ -892,7 +892,7 @@
         <v>1645</v>
       </c>
       <c r="M5" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N5" t="str">
         <v>1835</v>
@@ -901,7 +901,7 @@
         <v>1735</v>
       </c>
       <c r="P5" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q5" t="str">
         <v>3:20</v>
@@ -996,28 +996,28 @@
         <v>DX 0077</v>
       </c>
       <c r="J6" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K6" t="str">
-        <v>KRP</v>
+        <v>0945</v>
       </c>
       <c r="L6" t="str">
-        <v>0945</v>
+        <v>0845</v>
       </c>
       <c r="M6" t="str">
-        <v>0845</v>
+        <v>CPH</v>
       </c>
       <c r="N6" t="str">
-        <v>CPH</v>
+        <v>1035</v>
       </c>
       <c r="O6" t="str">
-        <v>1035</v>
+        <v>0935</v>
       </c>
       <c r="P6" t="str">
-        <v>0935</v>
+        <v>DO4</v>
       </c>
       <c r="Q6" t="str">
-        <v>DO4</v>
+        <v/>
       </c>
       <c r="R6" t="str">
         <v/>
@@ -1035,19 +1035,19 @@
         <v/>
       </c>
       <c r="W6" t="str">
-        <v/>
+        <v>OYJRY</v>
       </c>
       <c r="X6" t="str">
-        <v>OYJRY</v>
+        <v/>
       </c>
       <c r="Y6" t="str">
         <v/>
       </c>
       <c r="Z6" t="str">
-        <v/>
+        <v>LETTHIILV</v>
       </c>
       <c r="AA6" t="str">
-        <v>LETTHIILV</v>
+        <v/>
       </c>
       <c r="AB6" t="str">
         <v/>
@@ -1100,16 +1100,16 @@
         <v/>
       </c>
       <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
         <v>DX80</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" t="str">
         <v>DX 0080</v>
       </c>
-      <c r="I7" t="str">
-        <v/>
-      </c>
       <c r="J7" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K7" t="str">
         <v>1445</v>
@@ -1118,7 +1118,7 @@
         <v>1345</v>
       </c>
       <c r="M7" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N7" t="str">
         <v>1535</v>
@@ -1127,7 +1127,7 @@
         <v>1435</v>
       </c>
       <c r="P7" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q7" t="str">
         <v/>
@@ -1213,16 +1213,16 @@
         <v/>
       </c>
       <c r="G8" t="str">
+        <v/>
+      </c>
+      <c r="H8" t="str">
         <v>DX83</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <v>DX 0083</v>
       </c>
-      <c r="I8" t="str">
-        <v/>
-      </c>
       <c r="J8" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K8" t="str">
         <v>1620</v>
@@ -1231,7 +1231,7 @@
         <v>1520</v>
       </c>
       <c r="M8" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="N8" t="str">
         <v>1710</v>
@@ -1240,7 +1240,7 @@
         <v>1610</v>
       </c>
       <c r="P8" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q8" t="str">
         <v/>
@@ -1320,22 +1320,22 @@
         <v/>
       </c>
       <c r="E9" t="str">
+        <v/>
+      </c>
+      <c r="F9" t="str">
         <v>1855</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <v>1755</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <v>DX82</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <v>DX 0082</v>
       </c>
-      <c r="I9" t="str">
-        <v/>
-      </c>
       <c r="J9" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K9" t="str">
         <v>1745</v>
@@ -1344,7 +1344,7 @@
         <v>1645</v>
       </c>
       <c r="M9" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N9" t="str">
         <v>1835</v>
@@ -1353,7 +1353,7 @@
         <v>1735</v>
       </c>
       <c r="P9" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q9" t="str">
         <v>3:20</v>
@@ -1413,10 +1413,10 @@
         <v>12:00</v>
       </c>
       <c r="AJ9" t="str">
+        <v/>
+      </c>
+      <c r="AK9" t="str">
         <v>0655+1</v>
-      </c>
-      <c r="AK9" t="str">
-        <v/>
       </c>
     </row>
     <row r="10">
@@ -1448,25 +1448,25 @@
         <v>OFF</v>
       </c>
       <c r="J10" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K10" t="str">
+        <v>0000</v>
+      </c>
+      <c r="L10" t="str">
+        <v>2300-1</v>
+      </c>
+      <c r="M10" t="str">
         <v>KRP</v>
       </c>
-      <c r="L10" t="str">
-        <v>0000</v>
-      </c>
-      <c r="M10" t="str">
-        <v>2300-1</v>
-      </c>
       <c r="N10" t="str">
-        <v>KRP</v>
+        <v>2400</v>
       </c>
       <c r="O10" t="str">
-        <v>2400</v>
+        <v>2300</v>
       </c>
       <c r="P10" t="str">
-        <v>2300</v>
+        <v/>
       </c>
       <c r="Q10" t="str">
         <v/>
@@ -1493,16 +1493,16 @@
         <v/>
       </c>
       <c r="Y10" t="str">
-        <v/>
+        <v>ILV</v>
       </c>
       <c r="Z10" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AA10" t="str">
-        <v>ILV</v>
+        <v/>
       </c>
       <c r="AB10" t="str">
-        <v>-</v>
+        <v/>
       </c>
       <c r="AC10" t="str">
         <v/>
@@ -1561,25 +1561,25 @@
         <v>OFF</v>
       </c>
       <c r="J11" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K11" t="str">
+        <v>0000</v>
+      </c>
+      <c r="L11" t="str">
+        <v>2300-1</v>
+      </c>
+      <c r="M11" t="str">
         <v>KRP</v>
       </c>
-      <c r="L11" t="str">
-        <v>0000</v>
-      </c>
-      <c r="M11" t="str">
-        <v>2300-1</v>
-      </c>
       <c r="N11" t="str">
-        <v>KRP</v>
+        <v>2400</v>
       </c>
       <c r="O11" t="str">
-        <v>2400</v>
+        <v>2300</v>
       </c>
       <c r="P11" t="str">
-        <v>2300</v>
+        <v/>
       </c>
       <c r="Q11" t="str">
         <v/>
@@ -1606,19 +1606,19 @@
         <v/>
       </c>
       <c r="Y11" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="Z11" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="AA11" t="str">
         <v>|</v>
       </c>
       <c r="AB11" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AC11" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AD11" t="str">
         <v/>
@@ -1674,25 +1674,25 @@
         <v>OFF</v>
       </c>
       <c r="J12" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K12" t="str">
+        <v>0000</v>
+      </c>
+      <c r="L12" t="str">
+        <v>2300-1</v>
+      </c>
+      <c r="M12" t="str">
         <v>KRP</v>
       </c>
-      <c r="L12" t="str">
-        <v>0000</v>
-      </c>
-      <c r="M12" t="str">
-        <v>2300-1</v>
-      </c>
       <c r="N12" t="str">
-        <v>KRP</v>
+        <v>2400</v>
       </c>
       <c r="O12" t="str">
-        <v>2400</v>
+        <v>2300</v>
       </c>
       <c r="P12" t="str">
-        <v>2300</v>
+        <v/>
       </c>
       <c r="Q12" t="str">
         <v/>
@@ -1719,19 +1719,19 @@
         <v/>
       </c>
       <c r="Y12" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="Z12" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="AA12" t="str">
         <v>|</v>
       </c>
       <c r="AB12" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AC12" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AD12" t="str">
         <v/>
@@ -1787,43 +1787,43 @@
         <v>SBY</v>
       </c>
       <c r="J13" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K13" t="str">
+        <v>0600</v>
+      </c>
+      <c r="L13" t="str">
+        <v>0500</v>
+      </c>
+      <c r="M13" t="str">
         <v>KRP</v>
       </c>
-      <c r="L13" t="str">
-        <v>0600</v>
-      </c>
-      <c r="M13" t="str">
-        <v>0500</v>
-      </c>
       <c r="N13" t="str">
-        <v>KRP</v>
+        <v>1800</v>
       </c>
       <c r="O13" t="str">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="P13" t="str">
-        <v>1700</v>
+        <v>0:00</v>
       </c>
       <c r="Q13" t="str">
         <v/>
       </c>
       <c r="R13" t="str">
-        <v>0:00</v>
+        <v/>
       </c>
       <c r="S13" t="str">
-        <v/>
+        <v>3:00</v>
       </c>
       <c r="T13" t="str">
-        <v/>
+        <v>0</v>
       </c>
       <c r="U13" t="str">
-        <v>3:00</v>
+        <v/>
       </c>
       <c r="V13" t="str">
-        <v>0</v>
+        <v/>
       </c>
       <c r="W13" t="str">
         <v/>
@@ -1832,19 +1832,19 @@
         <v/>
       </c>
       <c r="Y13" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="Z13" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="AA13" t="str">
         <v>|</v>
       </c>
       <c r="AB13" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AC13" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AD13" t="str">
         <v/>
@@ -1859,16 +1859,16 @@
         <v/>
       </c>
       <c r="AH13" t="str">
-        <v/>
+        <v>4:00</v>
       </c>
       <c r="AI13" t="str">
-        <v/>
+        <v>0600+1</v>
       </c>
       <c r="AJ13" t="str">
-        <v>4:00</v>
+        <v/>
       </c>
       <c r="AK13" t="str">
-        <v>0600+1</v>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -1900,43 +1900,43 @@
         <v>SBY</v>
       </c>
       <c r="J14" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K14" t="str">
+        <v>0600</v>
+      </c>
+      <c r="L14" t="str">
+        <v>0500</v>
+      </c>
+      <c r="M14" t="str">
         <v>KRP</v>
       </c>
-      <c r="L14" t="str">
-        <v>0600</v>
-      </c>
-      <c r="M14" t="str">
-        <v>0500</v>
-      </c>
       <c r="N14" t="str">
-        <v>KRP</v>
+        <v>1800</v>
       </c>
       <c r="O14" t="str">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="P14" t="str">
-        <v>1700</v>
+        <v>0:00</v>
       </c>
       <c r="Q14" t="str">
         <v/>
       </c>
       <c r="R14" t="str">
-        <v>0:00</v>
+        <v/>
       </c>
       <c r="S14" t="str">
-        <v/>
+        <v>3:00</v>
       </c>
       <c r="T14" t="str">
-        <v/>
+        <v>0</v>
       </c>
       <c r="U14" t="str">
-        <v>3:00</v>
+        <v/>
       </c>
       <c r="V14" t="str">
-        <v>0</v>
+        <v/>
       </c>
       <c r="W14" t="str">
         <v/>
@@ -1945,19 +1945,19 @@
         <v/>
       </c>
       <c r="Y14" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="Z14" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="AA14" t="str">
         <v>|</v>
       </c>
       <c r="AB14" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AC14" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AD14" t="str">
         <v/>
@@ -1972,16 +1972,16 @@
         <v/>
       </c>
       <c r="AH14" t="str">
-        <v/>
+        <v>4:00</v>
       </c>
       <c r="AI14" t="str">
-        <v/>
+        <v>0600+1</v>
       </c>
       <c r="AJ14" t="str">
-        <v>4:00</v>
+        <v/>
       </c>
       <c r="AK14" t="str">
-        <v>0600+1</v>
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -2013,28 +2013,28 @@
         <v>DX 0077</v>
       </c>
       <c r="J15" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K15" t="str">
-        <v>KRP</v>
+        <v>0945</v>
       </c>
       <c r="L15" t="str">
-        <v>0945</v>
+        <v>0845</v>
       </c>
       <c r="M15" t="str">
-        <v>0845</v>
+        <v>CPH</v>
       </c>
       <c r="N15" t="str">
-        <v>CPH</v>
+        <v>1035</v>
       </c>
       <c r="O15" t="str">
-        <v>1035</v>
+        <v>0935</v>
       </c>
       <c r="P15" t="str">
-        <v>0935</v>
+        <v>DO4</v>
       </c>
       <c r="Q15" t="str">
-        <v>DO4</v>
+        <v/>
       </c>
       <c r="R15" t="str">
         <v/>
@@ -2052,25 +2052,25 @@
         <v/>
       </c>
       <c r="W15" t="str">
-        <v/>
+        <v>OYJRY</v>
       </c>
       <c r="X15" t="str">
-        <v>OYJRY</v>
+        <v/>
       </c>
       <c r="Y15" t="str">
         <v/>
       </c>
       <c r="Z15" t="str">
-        <v/>
+        <v>HANTHIILV</v>
       </c>
       <c r="AA15" t="str">
-        <v>HANTHIILV</v>
+        <v>CP (PIC)FOCA</v>
       </c>
       <c r="AB15" t="str">
         <v/>
       </c>
       <c r="AC15" t="str">
-        <v>CP (PIC)FOCA</v>
+        <v/>
       </c>
       <c r="AD15" t="str">
         <v/>
@@ -2117,16 +2117,16 @@
         <v/>
       </c>
       <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16" t="str">
         <v>DX80</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" t="str">
         <v>DX 0080</v>
       </c>
-      <c r="I16" t="str">
-        <v/>
-      </c>
       <c r="J16" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K16" t="str">
         <v>1445</v>
@@ -2135,7 +2135,7 @@
         <v>1345</v>
       </c>
       <c r="M16" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N16" t="str">
         <v>1535</v>
@@ -2144,7 +2144,7 @@
         <v>1435</v>
       </c>
       <c r="P16" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q16" t="str">
         <v/>
@@ -2230,16 +2230,16 @@
         <v/>
       </c>
       <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="str">
         <v>DX83</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" t="str">
         <v>DX 0083</v>
       </c>
-      <c r="I17" t="str">
-        <v/>
-      </c>
       <c r="J17" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K17" t="str">
         <v>1620</v>
@@ -2248,7 +2248,7 @@
         <v>1520</v>
       </c>
       <c r="M17" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="N17" t="str">
         <v>1710</v>
@@ -2257,7 +2257,7 @@
         <v>1610</v>
       </c>
       <c r="P17" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q17" t="str">
         <v/>
@@ -2337,22 +2337,22 @@
         <v/>
       </c>
       <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
         <v>1855</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <v>1755</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <v>DX82</v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" t="str">
         <v>DX 0082</v>
       </c>
-      <c r="I18" t="str">
-        <v/>
-      </c>
       <c r="J18" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K18" t="str">
         <v>1745</v>
@@ -2361,7 +2361,7 @@
         <v>1645</v>
       </c>
       <c r="M18" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N18" t="str">
         <v>1835</v>
@@ -2370,7 +2370,7 @@
         <v>1735</v>
       </c>
       <c r="P18" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q18" t="str">
         <v>3:20</v>
@@ -2430,10 +2430,10 @@
         <v>12:00</v>
       </c>
       <c r="AJ18" t="str">
+        <v/>
+      </c>
+      <c r="AK18" t="str">
         <v>0655+1</v>
-      </c>
-      <c r="AK18" t="str">
-        <v/>
       </c>
     </row>
     <row r="19">
@@ -2465,25 +2465,25 @@
         <v>OFF</v>
       </c>
       <c r="J19" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K19" t="str">
+        <v>0000</v>
+      </c>
+      <c r="L19" t="str">
+        <v>2300-1</v>
+      </c>
+      <c r="M19" t="str">
         <v>KRP</v>
       </c>
-      <c r="L19" t="str">
-        <v>0000</v>
-      </c>
-      <c r="M19" t="str">
-        <v>2300-1</v>
-      </c>
       <c r="N19" t="str">
-        <v>KRP</v>
+        <v>2400</v>
       </c>
       <c r="O19" t="str">
-        <v>2400</v>
+        <v>2300</v>
       </c>
       <c r="P19" t="str">
-        <v>2300</v>
+        <v/>
       </c>
       <c r="Q19" t="str">
         <v/>
@@ -2510,16 +2510,16 @@
         <v/>
       </c>
       <c r="Y19" t="str">
-        <v/>
+        <v>ILV</v>
       </c>
       <c r="Z19" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AA19" t="str">
-        <v>ILV</v>
+        <v/>
       </c>
       <c r="AB19" t="str">
-        <v>-</v>
+        <v/>
       </c>
       <c r="AC19" t="str">
         <v/>
@@ -2578,25 +2578,25 @@
         <v>OFF</v>
       </c>
       <c r="J20" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K20" t="str">
+        <v>0000</v>
+      </c>
+      <c r="L20" t="str">
+        <v>2300-1</v>
+      </c>
+      <c r="M20" t="str">
         <v>KRP</v>
       </c>
-      <c r="L20" t="str">
-        <v>0000</v>
-      </c>
-      <c r="M20" t="str">
-        <v>2300-1</v>
-      </c>
       <c r="N20" t="str">
-        <v>KRP</v>
+        <v>2400</v>
       </c>
       <c r="O20" t="str">
-        <v>2400</v>
+        <v>2300</v>
       </c>
       <c r="P20" t="str">
-        <v>2300</v>
+        <v/>
       </c>
       <c r="Q20" t="str">
         <v/>
@@ -2623,19 +2623,19 @@
         <v/>
       </c>
       <c r="Y20" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="Z20" t="str">
-        <v/>
+        <v>|</v>
       </c>
       <c r="AA20" t="str">
         <v>|</v>
       </c>
       <c r="AB20" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AC20" t="str">
-        <v>|</v>
+        <v/>
       </c>
       <c r="AD20" t="str">
         <v/>
@@ -2691,28 +2691,28 @@
         <v>DX 0073</v>
       </c>
       <c r="J21" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K21" t="str">
-        <v>KRP</v>
+        <v>0700</v>
       </c>
       <c r="L21" t="str">
-        <v>0700</v>
+        <v>0600</v>
       </c>
       <c r="M21" t="str">
-        <v>0600</v>
+        <v>CPH</v>
       </c>
       <c r="N21" t="str">
-        <v>CPH</v>
+        <v>0750</v>
       </c>
       <c r="O21" t="str">
-        <v>0750</v>
+        <v>0650</v>
       </c>
       <c r="P21" t="str">
-        <v>0650</v>
+        <v>DO4</v>
       </c>
       <c r="Q21" t="str">
-        <v>DO4</v>
+        <v/>
       </c>
       <c r="R21" t="str">
         <v/>
@@ -2730,25 +2730,25 @@
         <v/>
       </c>
       <c r="W21" t="str">
-        <v/>
+        <v>OYJRY</v>
       </c>
       <c r="X21" t="str">
-        <v>OYJRY</v>
+        <v/>
       </c>
       <c r="Y21" t="str">
         <v/>
       </c>
       <c r="Z21" t="str">
-        <v/>
+        <v>HANBROILV</v>
       </c>
       <c r="AA21" t="str">
-        <v>HANBROILV</v>
+        <v>CP (PIC)FOCA</v>
       </c>
       <c r="AB21" t="str">
         <v/>
       </c>
       <c r="AC21" t="str">
-        <v>CP (PIC)FOCA</v>
+        <v/>
       </c>
       <c r="AD21" t="str">
         <v/>
@@ -2795,16 +2795,16 @@
         <v/>
       </c>
       <c r="G22" t="str">
+        <v/>
+      </c>
+      <c r="H22" t="str">
         <v>DX74</v>
       </c>
-      <c r="H22" t="str">
+      <c r="I22" t="str">
         <v>DX 0074</v>
       </c>
-      <c r="I22" t="str">
-        <v/>
-      </c>
       <c r="J22" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K22" t="str">
         <v>0820</v>
@@ -2813,7 +2813,7 @@
         <v>0720</v>
       </c>
       <c r="M22" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N22" t="str">
         <v>0910</v>
@@ -2822,7 +2822,7 @@
         <v>0810</v>
       </c>
       <c r="P22" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q22" t="str">
         <v/>
@@ -2908,16 +2908,16 @@
         <v/>
       </c>
       <c r="G23" t="str">
+        <v/>
+      </c>
+      <c r="H23" t="str">
         <v>DX77</v>
       </c>
-      <c r="H23" t="str">
+      <c r="I23" t="str">
         <v>DX 0077</v>
       </c>
-      <c r="I23" t="str">
-        <v/>
-      </c>
       <c r="J23" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K23" t="str">
         <v>0945</v>
@@ -2926,7 +2926,7 @@
         <v>0845</v>
       </c>
       <c r="M23" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="N23" t="str">
         <v>1035</v>
@@ -2935,7 +2935,7 @@
         <v>0935</v>
       </c>
       <c r="P23" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q23" t="str">
         <v/>
@@ -3015,22 +3015,22 @@
         <v/>
       </c>
       <c r="E24" t="str">
+        <v/>
+      </c>
+      <c r="F24" t="str">
         <v>1530</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <v>1430</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <v>DX80</v>
       </c>
-      <c r="H24" t="str">
+      <c r="I24" t="str">
         <v>DX 0080</v>
       </c>
-      <c r="I24" t="str">
-        <v/>
-      </c>
       <c r="J24" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K24" t="str">
         <v>1415</v>
@@ -3039,7 +3039,7 @@
         <v>1315</v>
       </c>
       <c r="M24" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N24" t="str">
         <v>1510</v>
@@ -3048,7 +3048,7 @@
         <v>1410</v>
       </c>
       <c r="P24" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q24" t="str">
         <v>3:25</v>
@@ -3143,28 +3143,28 @@
         <v>DX 0073</v>
       </c>
       <c r="J25" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K25" t="str">
-        <v>KRP</v>
+        <v>0700</v>
       </c>
       <c r="L25" t="str">
-        <v>0700</v>
+        <v>0600</v>
       </c>
       <c r="M25" t="str">
-        <v>0600</v>
+        <v>CPH</v>
       </c>
       <c r="N25" t="str">
-        <v>CPH</v>
+        <v>0750</v>
       </c>
       <c r="O25" t="str">
-        <v>0750</v>
+        <v>0650</v>
       </c>
       <c r="P25" t="str">
-        <v>0650</v>
+        <v>DO4</v>
       </c>
       <c r="Q25" t="str">
-        <v>DO4</v>
+        <v/>
       </c>
       <c r="R25" t="str">
         <v/>
@@ -3182,25 +3182,25 @@
         <v/>
       </c>
       <c r="W25" t="str">
-        <v/>
+        <v>OYJRY</v>
       </c>
       <c r="X25" t="str">
-        <v>OYJRY</v>
+        <v/>
       </c>
       <c r="Y25" t="str">
         <v/>
       </c>
       <c r="Z25" t="str">
-        <v/>
+        <v>TIOTHIILV</v>
       </c>
       <c r="AA25" t="str">
-        <v>TIOTHIILV</v>
+        <v>CP (PIC)FOCA</v>
       </c>
       <c r="AB25" t="str">
         <v/>
       </c>
       <c r="AC25" t="str">
-        <v>CP (PIC)FOCA</v>
+        <v/>
       </c>
       <c r="AD25" t="str">
         <v/>
@@ -3247,16 +3247,16 @@
         <v/>
       </c>
       <c r="G26" t="str">
+        <v/>
+      </c>
+      <c r="H26" t="str">
         <v>DX74</v>
       </c>
-      <c r="H26" t="str">
+      <c r="I26" t="str">
         <v>DX 0074</v>
       </c>
-      <c r="I26" t="str">
-        <v/>
-      </c>
       <c r="J26" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K26" t="str">
         <v>0820</v>
@@ -3265,7 +3265,7 @@
         <v>0720</v>
       </c>
       <c r="M26" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N26" t="str">
         <v>0910</v>
@@ -3274,7 +3274,7 @@
         <v>0810</v>
       </c>
       <c r="P26" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q26" t="str">
         <v/>
@@ -3360,16 +3360,16 @@
         <v/>
       </c>
       <c r="G27" t="str">
+        <v/>
+      </c>
+      <c r="H27" t="str">
         <v>DX77</v>
       </c>
-      <c r="H27" t="str">
+      <c r="I27" t="str">
         <v>DX 0077</v>
       </c>
-      <c r="I27" t="str">
-        <v/>
-      </c>
       <c r="J27" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K27" t="str">
         <v>0945</v>
@@ -3378,7 +3378,7 @@
         <v>0845</v>
       </c>
       <c r="M27" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="N27" t="str">
         <v>1035</v>
@@ -3387,7 +3387,7 @@
         <v>0935</v>
       </c>
       <c r="P27" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q27" t="str">
         <v/>
@@ -3467,22 +3467,22 @@
         <v/>
       </c>
       <c r="E28" t="str">
+        <v/>
+      </c>
+      <c r="F28" t="str">
         <v>1600</v>
       </c>
-      <c r="F28" t="str">
+      <c r="G28" t="str">
         <v>1500</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <v>DX80</v>
       </c>
-      <c r="H28" t="str">
+      <c r="I28" t="str">
         <v>DX 0080</v>
       </c>
-      <c r="I28" t="str">
-        <v/>
-      </c>
       <c r="J28" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K28" t="str">
         <v>1445</v>
@@ -3491,7 +3491,7 @@
         <v>1345</v>
       </c>
       <c r="M28" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N28" t="str">
         <v>1540</v>
@@ -3500,7 +3500,7 @@
         <v>1440</v>
       </c>
       <c r="P28" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q28" t="str">
         <v>3:25</v>
@@ -3595,25 +3595,25 @@
         <v>Comapany Car</v>
       </c>
       <c r="J29" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K29" t="str">
-        <v>KRP</v>
+        <v>0655</v>
       </c>
       <c r="L29" t="str">
-        <v>0655</v>
+        <v>0555</v>
       </c>
       <c r="M29" t="str">
-        <v>0555</v>
+        <v>EBJ</v>
       </c>
       <c r="N29" t="str">
-        <v>EBJ</v>
+        <v>0820</v>
       </c>
       <c r="O29" t="str">
-        <v>0820</v>
+        <v>0720</v>
       </c>
       <c r="P29" t="str">
-        <v>0720</v>
+        <v/>
       </c>
       <c r="Q29" t="str">
         <v/>
@@ -3687,28 +3687,28 @@
         <v/>
       </c>
       <c r="C30" t="str">
+        <v/>
+      </c>
+      <c r="D30" t="str">
         <v>0820</v>
       </c>
-      <c r="D30" t="str">
+      <c r="E30" t="str">
         <v>0720</v>
       </c>
-      <c r="E30" t="str">
-        <v/>
-      </c>
       <c r="F30" t="str">
         <v/>
       </c>
       <c r="G30" t="str">
+        <v/>
+      </c>
+      <c r="H30" t="str">
         <v>DX21</v>
       </c>
-      <c r="H30" t="str">
+      <c r="I30" t="str">
         <v>DX 0021</v>
       </c>
-      <c r="I30" t="str">
-        <v/>
-      </c>
       <c r="J30" t="str">
-        <v/>
+        <v>EBJ</v>
       </c>
       <c r="K30" t="str">
         <v>0920</v>
@@ -3717,7 +3717,7 @@
         <v>0820</v>
       </c>
       <c r="M30" t="str">
-        <v/>
+        <v>SVG</v>
       </c>
       <c r="N30" t="str">
         <v>1030</v>
@@ -3726,7 +3726,7 @@
         <v>0930</v>
       </c>
       <c r="P30" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q30" t="str">
         <v/>
@@ -3759,10 +3759,10 @@
         <v>HANTHIILV</v>
       </c>
       <c r="AA30" t="str">
-        <v/>
+        <v>CP (PIC)FOCA</v>
       </c>
       <c r="AB30" t="str">
-        <v>CP (PIC)FOCA</v>
+        <v/>
       </c>
       <c r="AC30" t="str">
         <v/>
@@ -3812,16 +3812,16 @@
         <v/>
       </c>
       <c r="G31" t="str">
+        <v/>
+      </c>
+      <c r="H31" t="str">
         <v>DX22</v>
       </c>
-      <c r="H31" t="str">
+      <c r="I31" t="str">
         <v>DX 0022</v>
       </c>
-      <c r="I31" t="str">
-        <v/>
-      </c>
       <c r="J31" t="str">
-        <v/>
+        <v>SVG</v>
       </c>
       <c r="K31" t="str">
         <v>1100</v>
@@ -3830,7 +3830,7 @@
         <v>1000</v>
       </c>
       <c r="M31" t="str">
-        <v/>
+        <v>EBJ</v>
       </c>
       <c r="N31" t="str">
         <v>1210</v>
@@ -3839,7 +3839,7 @@
         <v>1110</v>
       </c>
       <c r="P31" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q31" t="str">
         <v/>
@@ -3910,31 +3910,31 @@
         <v/>
       </c>
       <c r="B32" t="str">
+        <v/>
+      </c>
+      <c r="C32" t="str">
         <v>DH</v>
       </c>
-      <c r="C32" t="str">
-        <v/>
-      </c>
       <c r="D32" t="str">
         <v/>
       </c>
       <c r="E32" t="str">
+        <v/>
+      </c>
+      <c r="F32" t="str">
         <v>1410</v>
       </c>
-      <c r="F32" t="str">
+      <c r="G32" t="str">
         <v>1310</v>
       </c>
-      <c r="G32" t="str">
+      <c r="H32" t="str">
         <v>CAR</v>
       </c>
-      <c r="H32" t="str">
+      <c r="I32" t="str">
         <v>Company Car</v>
       </c>
-      <c r="I32" t="str">
-        <v/>
-      </c>
       <c r="J32" t="str">
-        <v/>
+        <v>EBJ</v>
       </c>
       <c r="K32" t="str">
         <v>1230</v>
@@ -3943,7 +3943,7 @@
         <v>1130</v>
       </c>
       <c r="M32" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N32" t="str">
         <v>1410</v>
@@ -3952,22 +3952,22 @@
         <v>1310</v>
       </c>
       <c r="P32" t="str">
-        <v/>
+        <v>2:20</v>
       </c>
       <c r="Q32" t="str">
-        <v>2:20</v>
+        <v/>
       </c>
       <c r="R32" t="str">
         <v/>
       </c>
       <c r="S32" t="str">
-        <v/>
+        <v>7:15</v>
       </c>
       <c r="T32" t="str">
-        <v>7:15</v>
+        <v>0</v>
       </c>
       <c r="U32" t="str">
-        <v>0</v>
+        <v/>
       </c>
       <c r="V32" t="str">
         <v/>
@@ -4000,16 +4000,16 @@
         <v/>
       </c>
       <c r="AF32" t="str">
-        <v/>
+        <v>5:15</v>
       </c>
       <c r="AG32" t="str">
-        <v>5:15</v>
+        <v>13:00</v>
       </c>
       <c r="AH32" t="str">
-        <v>13:00</v>
+        <v>0210+1</v>
       </c>
       <c r="AI32" t="str">
-        <v>0210+1</v>
+        <v/>
       </c>
       <c r="AJ32" t="str">
         <v/>
@@ -4047,28 +4047,28 @@
         <v>DX 0079</v>
       </c>
       <c r="J33" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K33" t="str">
-        <v>KRP</v>
+        <v>1145</v>
       </c>
       <c r="L33" t="str">
-        <v>1145</v>
+        <v>1045</v>
       </c>
       <c r="M33" t="str">
-        <v>1045</v>
+        <v>CPH</v>
       </c>
       <c r="N33" t="str">
-        <v>CPH</v>
+        <v>1235</v>
       </c>
       <c r="O33" t="str">
-        <v>1235</v>
+        <v>1135</v>
       </c>
       <c r="P33" t="str">
-        <v>1135</v>
+        <v>DO4</v>
       </c>
       <c r="Q33" t="str">
-        <v>DO4</v>
+        <v/>
       </c>
       <c r="R33" t="str">
         <v/>
@@ -4086,25 +4086,25 @@
         <v/>
       </c>
       <c r="W33" t="str">
-        <v/>
+        <v>OYJRY</v>
       </c>
       <c r="X33" t="str">
-        <v>OYJRY</v>
+        <v/>
       </c>
       <c r="Y33" t="str">
         <v/>
       </c>
       <c r="Z33" t="str">
-        <v/>
+        <v>HANBROILV</v>
       </c>
       <c r="AA33" t="str">
-        <v>HANBROILV</v>
+        <v>CP (PIC)FOCA</v>
       </c>
       <c r="AB33" t="str">
         <v/>
       </c>
       <c r="AC33" t="str">
-        <v>CP (PIC)FOCA</v>
+        <v/>
       </c>
       <c r="AD33" t="str">
         <v/>
@@ -4151,16 +4151,16 @@
         <v/>
       </c>
       <c r="G34" t="str">
+        <v/>
+      </c>
+      <c r="H34" t="str">
         <v>DX82</v>
       </c>
-      <c r="H34" t="str">
+      <c r="I34" t="str">
         <v>DX 0082</v>
       </c>
-      <c r="I34" t="str">
-        <v/>
-      </c>
       <c r="J34" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K34" t="str">
         <v>1700</v>
@@ -4169,7 +4169,7 @@
         <v>1600</v>
       </c>
       <c r="M34" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N34" t="str">
         <v>1750</v>
@@ -4178,7 +4178,7 @@
         <v>1650</v>
       </c>
       <c r="P34" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q34" t="str">
         <v/>
@@ -4264,16 +4264,16 @@
         <v/>
       </c>
       <c r="G35" t="str">
+        <v/>
+      </c>
+      <c r="H35" t="str">
         <v>DX85</v>
       </c>
-      <c r="H35" t="str">
+      <c r="I35" t="str">
         <v>DX 0085</v>
       </c>
-      <c r="I35" t="str">
-        <v/>
-      </c>
       <c r="J35" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="K35" t="str">
         <v>1820</v>
@@ -4282,7 +4282,7 @@
         <v>1720</v>
       </c>
       <c r="M35" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="N35" t="str">
         <v>1910</v>
@@ -4291,7 +4291,7 @@
         <v>1810</v>
       </c>
       <c r="P35" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q35" t="str">
         <v/>
@@ -4371,22 +4371,22 @@
         <v/>
       </c>
       <c r="E36" t="str">
+        <v/>
+      </c>
+      <c r="F36" t="str">
         <v>2050</v>
       </c>
-      <c r="F36" t="str">
+      <c r="G36" t="str">
         <v>1950</v>
       </c>
-      <c r="G36" t="str">
+      <c r="H36" t="str">
         <v>DX86</v>
       </c>
-      <c r="H36" t="str">
+      <c r="I36" t="str">
         <v>DX 0086</v>
       </c>
-      <c r="I36" t="str">
-        <v/>
-      </c>
       <c r="J36" t="str">
-        <v/>
+        <v>CPH</v>
       </c>
       <c r="K36" t="str">
         <v>1940</v>
@@ -4395,7 +4395,7 @@
         <v>1840</v>
       </c>
       <c r="M36" t="str">
-        <v/>
+        <v>KRP</v>
       </c>
       <c r="N36" t="str">
         <v>2030</v>
@@ -4404,7 +4404,7 @@
         <v>1930</v>
       </c>
       <c r="P36" t="str">
-        <v/>
+        <v>DO4</v>
       </c>
       <c r="Q36" t="str">
         <v>3:20</v>
@@ -4464,10 +4464,10 @@
         <v>12:00</v>
       </c>
       <c r="AJ36" t="str">
+        <v/>
+      </c>
+      <c r="AK36" t="str">
         <v>0850+1</v>
-      </c>
-      <c r="AK36" t="str">
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>